<commit_message>
joo kut sxhip gemaakt
</commit_message>
<xml_diff>
--- a/schaalmodel/schaalmodel.xlsx
+++ b/schaalmodel/schaalmodel.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/bjtvannuland_tudelft_nl/Documents/Bachelor MT jaar 1/Q4/Integratieproject 1/IP-26/schaalmodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC10487271D94BF05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18AD46F1-B5DC-4B79-ACBD-65CB0D4EE4F5}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="11_F25DC773A252ABDACC10487271D94BF05ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D9FC1F1-8BD1-4366-AE6B-671EEF2CF488}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,19 +35,50 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+  <si>
+    <t>Volume dicht schip</t>
+  </si>
+  <si>
+    <t>Volume van holtes in schip</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Volume schot</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
   <si>
     <t>Schaal 1:1</t>
   </si>
   <si>
-    <t>Volume dicht schip</t>
-  </si>
-  <si>
-    <t>Volume van holtes in schip</t>
-  </si>
-  <si>
-    <t>Volume schot</t>
+    <t>A</t>
   </si>
   <si>
     <t>x</t>
@@ -59,50 +90,134 @@
     <t>z</t>
   </si>
   <si>
-    <t>A</t>
+    <t>dichtheid hout</t>
+  </si>
+  <si>
+    <t>dichtheid water</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
   <si>
     <t>massa schip</t>
   </si>
   <si>
-    <t>dichtheid hout</t>
-  </si>
-  <si>
     <t>deplacement</t>
   </si>
   <si>
-    <t>dichtheid water</t>
-  </si>
-  <si>
-    <t>g</t>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>COG_x</t>
+  </si>
+  <si>
+    <t>aantal container</t>
+  </si>
+  <si>
+    <t>F_c</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>COG_y</t>
+  </si>
+  <si>
+    <t>massa container</t>
+  </si>
+  <si>
+    <t>F_last</t>
+  </si>
+  <si>
+    <t>T_beladen</t>
   </si>
   <si>
     <t>COG_z</t>
   </si>
   <si>
-    <t>COG_y</t>
-  </si>
-  <si>
-    <t>COG_x</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Last</t>
+    <t>massa container totaal</t>
+  </si>
+  <si>
+    <t>arm_last</t>
   </si>
   <si>
     <t>volume</t>
+  </si>
+  <si>
+    <t>KG_last</t>
+  </si>
+  <si>
+    <t>I_LCG</t>
+  </si>
+  <si>
+    <t>LCB</t>
+  </si>
+  <si>
+    <t>#tiers</t>
+  </si>
+  <si>
+    <t>T_varend</t>
+  </si>
+  <si>
+    <t>LCG_c</t>
+  </si>
+  <si>
+    <t>#rijen</t>
+  </si>
+  <si>
+    <t>KG_container</t>
+  </si>
+  <si>
+    <t>#bays</t>
+  </si>
+  <si>
+    <t>KG_totaal</t>
+  </si>
+  <si>
+    <t>H_c</t>
+  </si>
+  <si>
+    <t>LCG</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>R_10</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>R_19</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>1:.270</t>
+  </si>
+  <si>
+    <t>1:270^3</t>
+  </si>
+  <si>
+    <t>schaalmodel</t>
+  </si>
+  <si>
+    <t>Kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,25 +529,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>38984000000000</v>
@@ -447,9 +563,9 @@
         <v>8256.5752530000009</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>-8573900000000</v>
@@ -463,8 +579,17 @@
       <c r="E2">
         <v>9103.4563479999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -480,8 +605,14 @@
       <c r="E3">
         <v>7430.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,7 +629,7 @@
         <v>7776.2420039999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -515,107 +646,546 @@
         <v>7734.4986929999995</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>450</v>
+        <f>450/1000000000</f>
+        <v>4.4999999999999998E-7</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8">
-        <f>1025/1000000000</f>
-        <v>1.0249999999999999E-6</v>
+        <f>1000/1000000000</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1">
-        <f>B9*E11*(-1)</f>
-        <v>-1.366873598295E+17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <f>B9*(-1)*J3</f>
+        <v>-136687359.82949999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8">
+        <f>190*1000</f>
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <f>B8*(B1+B2+B3+B4+B5)</f>
-        <v>1.393347195E+16</v>
+        <v>13933471.949999999</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <f>17211.293*1000000000</f>
         <v>17211293000000.002</v>
       </c>
       <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <f>E9*J3*E8</f>
+        <v>168842784.33000001</v>
+      </c>
+      <c r="J9" t="s">
         <v>17</v>
       </c>
-      <c r="H9">
-        <f>E9*E8</f>
-        <v>17641575.324999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <f>32.7*1000</f>
+        <v>32700.000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
-        <f>(B1*C1+B2*C2+B3*C3+B4*C4+B5*C5)/(B1+B2+B3+B4+B5)</f>
         <v>81243.539052239052</v>
       </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>14</v>
+      </c>
       <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <f>E10*E11*J3*-1</f>
+        <v>-15656760</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <f>15.9*1000</f>
+        <v>15900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>114000</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1">
+        <f>-H8-H9-H10</f>
+        <v>-16498664.500500023</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <f>10*1000</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8008.808560493595</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <f>E10*E11</f>
+        <v>1596000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12">
+        <f>13.5*1000</f>
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <f>K10+(2.7*1000)</f>
+        <v>18600</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14">
+        <f>175926.5*1000000000000</f>
+        <v>1.759265E+17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <f>83.49*1000</f>
+        <v>83490</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15">
+        <f>6.5*1000</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1">
+        <f>-1*(H8*B10+H9*B15+H11*H12)/(H10)</f>
+        <v>176855.69918038708</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <f>K10+H15*H18/2</f>
+        <v>18490</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1">
+        <f>(H8*B12+H10*B17+H11*H14)/(H10+H8+H11)</f>
+        <v>10015.657798664946</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18">
+        <f>2.59*1000</f>
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1">
+        <f>(B10*H8+B16*H10+H12*H11)/(H11+H10+H8)</f>
+        <v>83490</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <f>K14/E9</f>
+        <v>10221.573707448939</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20">
+        <v>171957.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <f>6.208*1000</f>
+        <v>6208</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21">
+        <v>728415.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1">
+        <f>B21+B20-B18</f>
+        <v>6413.9159087839907</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24">
+        <v>270</v>
+      </c>
+      <c r="J24">
+        <f>270^3</f>
+        <v>19683000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1">
-        <f>(B1*D1+B2*D2+B3*D3+B4*D4+B5*D5)/(B1+B2+B3+B4+B5)</f>
-        <v>-3.6493281460033734E-11</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B26" s="1" cm="1">
+        <f t="array" ref="B26:B28">$B$10:B12/1000</f>
+        <v>81.243539052239058</v>
+      </c>
+      <c r="C26" s="1">
+        <f>B26/$H$24</f>
+        <v>0.30090199648977428</v>
+      </c>
+      <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="E11">
+      <c r="E26">
+        <v>-136687359.82949999</v>
+      </c>
+      <c r="F26">
+        <f>E26/$J$24/$J$26</f>
+        <v>-0.70789371284865099</v>
+      </c>
+      <c r="J26">
         <v>9.81</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <f>(B1*E1+B2*E2+B3*E3+B4*E4+B5*E5)/(B1+B2+B3+B4+B5)</f>
-        <v>8008.808560493595</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>19</v>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" ref="C27:C36" si="0">B27/$H$24</f>
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>168842784.33000001</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F39" si="1">E27/$J$24/$J$26</f>
+        <v>0.87442427475486462</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1">
+        <v>8.0088085604935948</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9662253927754054E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <v>-15656760</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>-8.1085200426764217E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" cm="1">
+        <f t="array" ref="B29:B36">$B$15:B22/1000</f>
+        <v>83.49</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30922222222222218</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29">
+        <v>-16498664.500500023</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>-8.5445361479449394E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="1">
+        <v>176.85569918038706</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.65502110807550762</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1">
+        <v>18.489999999999998</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8481481481481477E-2</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="1">
+        <v>10.015657798664947</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7095028883944246E-2</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="1">
+        <v>83.49</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30922222222222218</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10.22157370744894</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7857680397959038E-2</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="1">
+        <v>6.2080000000000002</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2992592592592592E-2</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6.4139159087839905</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3755244106607374E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38" s="1"/>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39" s="1"/>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>